<commit_message>
feedback from ACB change
</commit_message>
<xml_diff>
--- a/solar-panels/modular-panel/p2c/3_WORK/P2C_ReadMe.xlsx
+++ b/solar-panels/modular-panel/p2c/3_WORK/P2C_ReadMe.xlsx
@@ -1225,32 +1225,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1258,149 +1252,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1409,6 +1274,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
       <protection locked="0"/>
@@ -1445,6 +1316,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1454,23 +1334,143 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1635,7 +1635,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4959,50 +4959,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>49696</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>33129</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>21294</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>30697</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9442174" y="2343977"/>
-          <a:ext cx="8552381" cy="6209524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5366,55 +5322,55 @@
       <c r="K1" s="27"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="98"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="14"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="93"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="92"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="101"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="99"/>
       <c r="E3" s="15"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="95"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="93"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="102" t="s">
+      <c r="B4" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="103"/>
-      <c r="D4" s="104"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="102"/>
       <c r="E4" s="15"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="93"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="104"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="102"/>
       <c r="E5" s="15"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="95"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="93"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="114"/>
       <c r="E6" s="16"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -5423,101 +5379,101 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="79"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="81"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="117"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="89"/>
-      <c r="C8" s="105" t="s">
+      <c r="B8" s="88"/>
+      <c r="C8" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="131">
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="55">
         <v>43892</v>
       </c>
-      <c r="H8" s="87"/>
+      <c r="H8" s="56"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="90"/>
-      <c r="C9" s="106" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="132" t="s">
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="H9" s="133"/>
+      <c r="H9" s="58"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="90"/>
-      <c r="C10" s="105" t="s">
+      <c r="B10" s="89"/>
+      <c r="C10" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="75">
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="59">
         <v>108153</v>
       </c>
-      <c r="H10" s="87"/>
+      <c r="H10" s="56"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="90"/>
-      <c r="C11" s="106" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="132" t="s">
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="133"/>
+      <c r="H11" s="58"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="90"/>
-      <c r="C12" s="105" t="s">
+      <c r="B12" s="89"/>
+      <c r="C12" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="87"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="103"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="56"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="90"/>
-      <c r="C13" s="108" t="s">
+      <c r="B13" s="89"/>
+      <c r="C13" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="108"/>
-      <c r="E13" s="108"/>
-      <c r="F13" s="108"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="109"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="107"/>
     </row>
     <row r="14" spans="1:17" s="25" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="110" t="s">
+      <c r="B14" s="89"/>
+      <c r="C14" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="85" t="s">
+      <c r="D14" s="109"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="123" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="86"/>
+      <c r="H14" s="67"/>
       <c r="I14" s="24"/>
       <c r="J14" s="24"/>
       <c r="K14" s="27"/>
@@ -5527,320 +5483,320 @@
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="1:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="90"/>
-      <c r="C15" s="88" t="s">
+      <c r="B15" s="89"/>
+      <c r="C15" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="128" t="s">
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="H15" s="129"/>
+      <c r="H15" s="61"/>
       <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="90"/>
-      <c r="C16" s="74" t="s">
+      <c r="B16" s="89"/>
+      <c r="C16" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="87"/>
+      <c r="H16" s="56"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="90"/>
-      <c r="C17" s="88" t="s">
+      <c r="B17" s="89"/>
+      <c r="C17" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64">
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62">
         <v>4</v>
       </c>
-      <c r="H17" s="65"/>
+      <c r="H17" s="63"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="90"/>
-      <c r="C18" s="74" t="s">
+      <c r="B18" s="89"/>
+      <c r="C18" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="112" t="s">
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="H18" s="113"/>
+      <c r="H18" s="111"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="91"/>
-      <c r="C19" s="88" t="s">
+      <c r="B19" s="90"/>
+      <c r="C19" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="130" t="s">
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="86"/>
+      <c r="H19" s="67"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="84"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="119"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="119"/>
+      <c r="H20" s="120"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75" t="s">
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="87"/>
+      <c r="H21" s="56"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64" t="s">
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="65"/>
+      <c r="H22" s="63"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75" t="s">
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="87"/>
+      <c r="H23" s="56"/>
     </row>
     <row r="24" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="64" t="s">
+      <c r="C24" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="128" t="s">
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="129"/>
+      <c r="H24" s="61"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75" t="s">
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="H25" s="87"/>
+      <c r="H25" s="56"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64" t="s">
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H26" s="65"/>
+      <c r="H26" s="63"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="66" t="s">
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="121" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="67"/>
+      <c r="H27" s="122"/>
       <c r="M27" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64" t="s">
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="H28" s="65"/>
+      <c r="H28" s="63"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="66" t="s">
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="121" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="67"/>
+      <c r="H29" s="122"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64" t="s">
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="65"/>
+      <c r="H30" s="63"/>
     </row>
     <row r="31" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="66" t="s">
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="67"/>
+      <c r="H31" s="122"/>
     </row>
     <row r="32" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="64" t="s">
+      <c r="C32" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64" t="s">
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="65"/>
+      <c r="H32" s="63"/>
     </row>
     <row r="33" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="66" t="s">
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="67"/>
+      <c r="H33" s="122"/>
     </row>
     <row r="34" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64" t="s">
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="H34" s="65"/>
+      <c r="H34" s="63"/>
     </row>
     <row r="35" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="66" t="s">
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="H35" s="67"/>
+      <c r="H35" s="122"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="65"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="63"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="67"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="121"/>
+      <c r="H37" s="122"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="61" t="s">
+      <c r="B38" s="127" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="63"/>
+      <c r="C38" s="128"/>
+      <c r="D38" s="128"/>
+      <c r="E38" s="128"/>
+      <c r="F38" s="128"/>
+      <c r="G38" s="128"/>
+      <c r="H38" s="129"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="21"/>
-      <c r="C39" s="69" t="s">
+      <c r="C39" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="70"/>
-      <c r="E39" s="71"/>
+      <c r="D39" s="131"/>
+      <c r="E39" s="132"/>
       <c r="F39" s="22" t="s">
         <v>4</v>
       </c>
@@ -5853,11 +5809,11 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="18"/>
-      <c r="C40" s="72" t="s">
+      <c r="C40" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
+      <c r="D40" s="133"/>
+      <c r="E40" s="133"/>
       <c r="F40" s="19" t="s">
         <v>13</v>
       </c>
@@ -5870,11 +5826,11 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
-      <c r="C41" s="115" t="s">
+      <c r="C41" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
       <c r="F41" s="12" t="s">
         <v>80</v>
       </c>
@@ -5887,11 +5843,11 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
-      <c r="C42" s="73" t="s">
+      <c r="C42" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="10" t="s">
         <v>101</v>
       </c>
@@ -5905,11 +5861,11 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="C43" s="68" t="s">
+      <c r="C43" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
       <c r="F43" s="32" t="s">
         <v>161</v>
       </c>
@@ -5922,11 +5878,11 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="31" t="s">
         <v>81</v>
       </c>
@@ -5940,11 +5896,11 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="68"/>
-      <c r="E45" s="68"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
       <c r="F45" s="53" t="s">
         <v>82</v>
       </c>
@@ -5958,11 +5914,11 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
       <c r="F46" s="52" t="s">
         <v>83</v>
       </c>
@@ -5976,11 +5932,11 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="68" t="s">
+      <c r="C47" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="68"/>
-      <c r="E47" s="68"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="53" t="s">
         <v>84</v>
       </c>
@@ -5994,11 +5950,11 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
-      <c r="C48" s="73" t="s">
+      <c r="C48" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
       <c r="F48" s="52" t="s">
         <v>85</v>
       </c>
@@ -6012,11 +5968,11 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="C49" s="68" t="s">
+      <c r="C49" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="68"/>
-      <c r="E49" s="68"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="72"/>
       <c r="F49" s="53" t="s">
         <v>86</v>
       </c>
@@ -6030,11 +5986,11 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
       <c r="F50" s="52" t="s">
         <v>87</v>
       </c>
@@ -6048,11 +6004,11 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
-      <c r="C51" s="68" t="s">
+      <c r="C51" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
       <c r="F51" s="53" t="s">
         <v>88</v>
       </c>
@@ -6066,11 +6022,11 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
-      <c r="C52" s="73" t="s">
+      <c r="C52" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="52" t="s">
         <v>89</v>
       </c>
@@ -6084,11 +6040,11 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
-      <c r="C53" s="68" t="s">
+      <c r="C53" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="68"/>
-      <c r="E53" s="68"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="72"/>
       <c r="F53" s="32" t="s">
         <v>102</v>
       </c>
@@ -6102,11 +6058,11 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
-      <c r="C54" s="73" t="s">
+      <c r="C54" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="73"/>
-      <c r="E54" s="73"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="71"/>
       <c r="F54" s="31" t="s">
         <v>116</v>
       </c>
@@ -6120,11 +6076,11 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
-      <c r="C55" s="55" t="s">
+      <c r="C55" s="124" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="56"/>
-      <c r="E55" s="57"/>
+      <c r="D55" s="125"/>
+      <c r="E55" s="126"/>
       <c r="F55" s="32" t="s">
         <v>117</v>
       </c>
@@ -6138,11 +6094,11 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
-      <c r="C56" s="73" t="s">
+      <c r="C56" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="31" t="s">
         <v>136</v>
       </c>
@@ -6156,11 +6112,11 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
-      <c r="C57" s="55" t="s">
+      <c r="C57" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="56"/>
-      <c r="E57" s="57"/>
+      <c r="D57" s="125"/>
+      <c r="E57" s="126"/>
       <c r="F57" s="32" t="s">
         <v>137</v>
       </c>
@@ -6174,11 +6130,11 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
-      <c r="C58" s="73" t="s">
+      <c r="C58" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
       <c r="F58" s="10" t="s">
         <v>93</v>
       </c>
@@ -6192,11 +6148,11 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
-      <c r="C59" s="68" t="s">
+      <c r="C59" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="D59" s="68"/>
-      <c r="E59" s="68"/>
+      <c r="D59" s="72"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="32" t="s">
         <v>99</v>
       </c>
@@ -6210,11 +6166,11 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
-      <c r="C60" s="58" t="s">
+      <c r="C60" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="D60" s="59"/>
-      <c r="E60" s="60"/>
+      <c r="D60" s="83"/>
+      <c r="E60" s="84"/>
       <c r="F60" s="10" t="s">
         <v>91</v>
       </c>
@@ -6229,11 +6185,11 @@
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="34"/>
-      <c r="C61" s="125" t="s">
+      <c r="C61" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="D61" s="126"/>
-      <c r="E61" s="127"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="87"/>
       <c r="F61" s="35" t="s">
         <v>112</v>
       </c>
@@ -6253,11 +6209,11 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
-      <c r="C62" s="58" t="s">
+      <c r="C62" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D62" s="59"/>
-      <c r="E62" s="60"/>
+      <c r="D62" s="83"/>
+      <c r="E62" s="84"/>
       <c r="F62" s="33" t="s">
         <v>151</v>
       </c>
@@ -6271,11 +6227,11 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B63" s="34"/>
-      <c r="C63" s="125" t="s">
+      <c r="C63" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="126"/>
-      <c r="E63" s="127"/>
+      <c r="D63" s="86"/>
+      <c r="E63" s="87"/>
       <c r="F63" s="35" t="s">
         <v>149</v>
       </c>
@@ -6289,11 +6245,11 @@
     </row>
     <row r="64" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="6"/>
-      <c r="C64" s="58" t="s">
+      <c r="C64" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="60"/>
+      <c r="D64" s="83"/>
+      <c r="E64" s="84"/>
       <c r="F64" s="33" t="s">
         <v>49</v>
       </c>
@@ -6304,42 +6260,42 @@
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="116" t="s">
+      <c r="B65" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="C65" s="117"/>
-      <c r="D65" s="117"/>
-      <c r="E65" s="117"/>
-      <c r="F65" s="117"/>
-      <c r="G65" s="117"/>
-      <c r="H65" s="118"/>
+      <c r="C65" s="74"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
+      <c r="F65" s="74"/>
+      <c r="G65" s="74"/>
+      <c r="H65" s="75"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="119"/>
-      <c r="C66" s="120"/>
-      <c r="D66" s="120"/>
-      <c r="E66" s="120"/>
-      <c r="F66" s="120"/>
-      <c r="G66" s="120"/>
-      <c r="H66" s="121"/>
+      <c r="B66" s="76"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="77"/>
+      <c r="F66" s="77"/>
+      <c r="G66" s="77"/>
+      <c r="H66" s="78"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="119"/>
-      <c r="C67" s="120"/>
-      <c r="D67" s="120"/>
-      <c r="E67" s="120"/>
-      <c r="F67" s="120"/>
-      <c r="G67" s="120"/>
-      <c r="H67" s="121"/>
+      <c r="B67" s="76"/>
+      <c r="C67" s="77"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="77"/>
+      <c r="F67" s="77"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="78"/>
     </row>
     <row r="68" spans="2:11" ht="238.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="122"/>
-      <c r="C68" s="123"/>
-      <c r="D68" s="123"/>
-      <c r="E68" s="123"/>
-      <c r="F68" s="123"/>
-      <c r="G68" s="123"/>
-      <c r="H68" s="124"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="80"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="80"/>
+      <c r="H68" s="81"/>
     </row>
     <row r="69" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="11"/>
@@ -6357,8 +6313,8 @@
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
-      <c r="G70" s="114"/>
-      <c r="H70" s="114"/>
+      <c r="G70" s="69"/>
+      <c r="H70" s="69"/>
       <c r="K70" s="27"/>
     </row>
     <row r="71" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6367,8 +6323,8 @@
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
-      <c r="G71" s="114"/>
-      <c r="H71" s="114"/>
+      <c r="G71" s="69"/>
+      <c r="H71" s="69"/>
       <c r="K71" s="27"/>
     </row>
     <row r="72" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6377,15 +6333,15 @@
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
-      <c r="G72" s="114"/>
-      <c r="H72" s="114"/>
+      <c r="G72" s="69"/>
+      <c r="H72" s="69"/>
       <c r="K72" s="27"/>
     </row>
     <row r="73" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="114"/>
-      <c r="C73" s="114"/>
-      <c r="D73" s="114"/>
-      <c r="E73" s="114"/>
+      <c r="B73" s="69"/>
+      <c r="C73" s="69"/>
+      <c r="D73" s="69"/>
+      <c r="E73" s="69"/>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
@@ -6471,9 +6427,9 @@
     </row>
     <row r="100" spans="2:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="11"/>
-      <c r="C100" s="94"/>
-      <c r="D100" s="94"/>
-      <c r="E100" s="94"/>
+      <c r="C100" s="68"/>
+      <c r="D100" s="68"/>
+      <c r="E100" s="68"/>
       <c r="F100" s="11"/>
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
@@ -6523,23 +6479,70 @@
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="B8:B19"/>
+    <mergeCell ref="G2:H5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
     <mergeCell ref="C100:E100"/>
     <mergeCell ref="B73:E73"/>
     <mergeCell ref="C41:E41"/>
@@ -6556,70 +6559,23 @@
     <mergeCell ref="G70:H72"/>
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="C56:E56"/>
-    <mergeCell ref="B8:B19"/>
-    <mergeCell ref="G2:H5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>